<commit_message>
update - 4/5/2023 - 3:54 -
</commit_message>
<xml_diff>
--- a/server/class-excel/841109222-12.xlsx
+++ b/server/class-excel/841109222-12.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Lớp Web 1</t>
   </si>
@@ -29,7 +29,10 @@
     <t>E-mail: thanhsang@sgu.edu.vn</t>
   </si>
   <si>
-    <t>Ngày tạo file: ngày 3 tháng 5, 2023</t>
+    <t>Ngày tạo file: ngày 4 tháng 5, 2023</t>
+  </si>
+  <si>
+    <t>Thông tin thí sinh</t>
   </si>
   <si>
     <t>Bài thi</t>
@@ -53,6 +56,9 @@
     <t>Web1-test</t>
   </si>
   <si>
+    <t xml:space="preserve">Test </t>
+  </si>
+  <si>
     <t>3121560033</t>
   </si>
   <si>
@@ -102,13 +108,46 @@
   </si>
   <si>
     <t>Subject</t>
+  </si>
+  <si>
+    <t>&lt;=0</t>
+  </si>
+  <si>
+    <t>&lt;=1</t>
+  </si>
+  <si>
+    <t>&lt;=2</t>
+  </si>
+  <si>
+    <t>&lt;=3</t>
+  </si>
+  <si>
+    <t>&lt;=4</t>
+  </si>
+  <si>
+    <t>&lt;=5</t>
+  </si>
+  <si>
+    <t>&lt;=6</t>
+  </si>
+  <si>
+    <t>&lt;=7</t>
+  </si>
+  <si>
+    <t>&lt;=8</t>
+  </si>
+  <si>
+    <t>&lt;=9</t>
+  </si>
+  <si>
+    <t>&lt;=10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -132,6 +171,11 @@
     </font>
     <font>
       <b/>
+      <color rgb="263895"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
     </font>
     <font>
@@ -140,6 +184,7 @@
     <font>
       <b/>
       <color rgb="cc2424"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="3">
@@ -155,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,11 +217,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="263895"/>
+      </left>
+      <right style="thin">
+        <color rgb="263895"/>
+      </right>
+      <top style="thin">
+        <color rgb="263895"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="263895"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -186,11 +246,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -575,131 +642,135 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="G6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="F10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -707,7 +778,7 @@
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -716,9 +787,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>